<commit_message>
Expect / ExpectRetern / ExpectThrown の補助メソッドを追加する (#6)
</commit_message>
<xml_diff>
--- a/FixtureBookTest/FixtureTest/Cast/Temp/TempConductorTest.xlsx
+++ b/FixtureBookTest/FixtureTest/Cast/Temp/TempConductorTest.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Expect" sheetId="5" r:id="rId1"/>
     <sheet name="ExpectReturn" sheetId="7" r:id="rId2"/>
     <sheet name="ExpectThrown" sheetId="6" r:id="rId3"/>
+    <sheet name="ValidateParameter" sheetId="8" r:id="rId4"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="61">
   <si>
     <t>A. テストケース</t>
     <phoneticPr fontId="3"/>
@@ -345,6 +346,92 @@
       <t>テイギ</t>
     </rPh>
     <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>ConfigException</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>ResourceKey</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>M_Fixture_Temp_Conductor_InvalidStatus</t>
+  </si>
+  <si>
+    <t>Message</t>
+  </si>
+  <si>
+    <t>%GetParamterAt%</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>Expect系メソッドを呼ぶ前にGetParamterAtメソッドを呼ぶと例外が発生する</t>
+    <rPh sb="6" eb="7">
+      <t>ケイ</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t>ヨ</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>マエ</t>
+    </rPh>
+    <rPh sb="34" eb="35">
+      <t>ヨ</t>
+    </rPh>
+    <rPh sb="37" eb="39">
+      <t>レイガイ</t>
+    </rPh>
+    <rPh sb="40" eb="42">
+      <t>ハッセイ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Expect系メソッドを呼ぶ前にValidateParamterAtメソッドを呼ぶと例外が発生する</t>
+    <rPh sb="6" eb="7">
+      <t>ケイ</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t>ヨ</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>マエ</t>
+    </rPh>
+    <rPh sb="39" eb="40">
+      <t>ヨ</t>
+    </rPh>
+    <rPh sb="42" eb="44">
+      <t>レイガイ</t>
+    </rPh>
+    <rPh sb="45" eb="47">
+      <t>ハッセイ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>%ValidateParamterAt%</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>GetParamterAtメソッドのインデックスがExpectの引数の数よりも多い場合は例外が発生する</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>M_Fixture_Temp_Conductor_InvalidParameterIndex</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>%(0)%</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>ValidateParamterAtメソッドのインデックスがExpectの引数の数よりも多い場合は例外が発生する</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>%(2)%</t>
+    <phoneticPr fontId="4"/>
   </si>
 </sst>
 </file>
@@ -838,8 +925,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="C91" sqref="C91"/>
+    <sheetView topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="A64" sqref="A64:XFD72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.6"/>
@@ -1218,7 +1305,7 @@
   <dimension ref="B2:E62"/>
   <sheetViews>
     <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+      <selection activeCell="A45" sqref="A45:XFD48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.6"/>
@@ -1487,7 +1574,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:XFD19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.6"/>
   <cols>
@@ -1613,4 +1702,226 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:E45"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.6"/>
+  <cols>
+    <col min="1" max="2" width="2.109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="2.77734375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="47.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="256" width="16.77734375" style="3" customWidth="1"/>
+    <col min="257" max="16384" width="8.88671875" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" s="1" customFormat="1">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5">
+      <c r="C4" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" s="2" customFormat="1">
+      <c r="B6" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5">
+      <c r="C7" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="5"/>
+    </row>
+    <row r="8" spans="2:5">
+      <c r="C8" s="6"/>
+      <c r="D8" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5">
+      <c r="C9" s="6"/>
+      <c r="D9" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" s="1" customFormat="1">
+      <c r="B11" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5">
+      <c r="C13" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" s="2" customFormat="1">
+      <c r="B15" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5">
+      <c r="C16" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" s="5"/>
+    </row>
+    <row r="17" spans="2:5">
+      <c r="C17" s="6"/>
+      <c r="D17" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5">
+      <c r="C18" s="6"/>
+      <c r="D18" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" s="1" customFormat="1">
+      <c r="B20" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5">
+      <c r="C22" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" s="2" customFormat="1">
+      <c r="B24" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5">
+      <c r="C25" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D25" s="5"/>
+    </row>
+    <row r="26" spans="2:5">
+      <c r="C26" s="6"/>
+      <c r="D26" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5">
+      <c r="C27" s="6"/>
+      <c r="D27" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" s="1" customFormat="1">
+      <c r="B29" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5">
+      <c r="C31" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" s="2" customFormat="1">
+      <c r="B33" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5">
+      <c r="C34" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34" s="5"/>
+    </row>
+    <row r="35" spans="2:5">
+      <c r="C35" s="6"/>
+      <c r="D35" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5">
+      <c r="C36" s="6"/>
+      <c r="D36" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5">
+      <c r="C38" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D38" s="5"/>
+    </row>
+    <row r="39" spans="2:5">
+      <c r="C39" s="6"/>
+      <c r="D39" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5">
+      <c r="C40" s="6"/>
+      <c r="D40" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" s="2" customFormat="1">
+      <c r="B42" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5">
+      <c r="C43" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D43" s="5"/>
+    </row>
+    <row r="44" spans="2:5">
+      <c r="C44" s="6"/>
+      <c r="D44" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E44" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5">
+      <c r="C45" s="6"/>
+      <c r="D45" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E45" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
GetParameterAt, ValidaterParameterAt 呼び出し時のエラーメッセージにtypoがある (#12)
</commit_message>
<xml_diff>
--- a/FixtureBookTest/FixtureTest/Cast/Temp/TempConductorTest.xlsx
+++ b/FixtureBookTest/FixtureTest/Cast/Temp/TempConductorTest.xlsx
@@ -362,11 +362,19 @@
     <t>Message</t>
   </si>
   <si>
-    <t>%GetParamterAt%</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>Expect系メソッドを呼ぶ前にGetParamterAtメソッドを呼ぶと例外が発生する</t>
+    <t>M_Fixture_Temp_Conductor_InvalidParameterIndex</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>%(0)%</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>%(2)%</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>Expect系メソッドを呼ぶ前にGetParameterAtメソッドを呼ぶと例外が発生する</t>
     <rPh sb="6" eb="7">
       <t>ケイ</t>
     </rPh>
@@ -376,19 +384,27 @@
     <rPh sb="14" eb="15">
       <t>マエ</t>
     </rPh>
-    <rPh sb="34" eb="35">
+    <rPh sb="35" eb="36">
       <t>ヨ</t>
     </rPh>
-    <rPh sb="37" eb="39">
+    <rPh sb="38" eb="40">
       <t>レイガイ</t>
     </rPh>
-    <rPh sb="40" eb="42">
+    <rPh sb="41" eb="43">
       <t>ハッセイ</t>
     </rPh>
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>Expect系メソッドを呼ぶ前にValidateParamterAtメソッドを呼ぶと例外が発生する</t>
+    <t>%GetParameterAt%</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>%ValidateParameterAt%</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>Expect系メソッドを呼ぶ前にValidateParameterAtメソッドを呼ぶと例外が発生する</t>
     <rPh sb="6" eb="7">
       <t>ケイ</t>
     </rPh>
@@ -398,40 +414,24 @@
     <rPh sb="14" eb="15">
       <t>マエ</t>
     </rPh>
-    <rPh sb="39" eb="40">
+    <rPh sb="40" eb="41">
       <t>ヨ</t>
     </rPh>
-    <rPh sb="42" eb="44">
+    <rPh sb="43" eb="45">
       <t>レイガイ</t>
     </rPh>
-    <rPh sb="45" eb="47">
+    <rPh sb="46" eb="48">
       <t>ハッセイ</t>
     </rPh>
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>%ValidateParamterAt%</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>GetParamterAtメソッドのインデックスがExpectの引数の数よりも多い場合は例外が発生する</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>M_Fixture_Temp_Conductor_InvalidParameterIndex</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>%(0)%</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>ValidateParamterAtメソッドのインデックスがExpectの引数の数よりも多い場合は例外が発生する</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>%(2)%</t>
-    <phoneticPr fontId="4"/>
+    <t>GetParameterAtメソッドのインデックスがExpectの引数の数よりも多い場合は例外が発生する</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>ValidateParameterAtメソッドのインデックスがExpectの引数の数よりも多い場合は例外が発生する</t>
+    <phoneticPr fontId="3"/>
   </si>
 </sst>
 </file>
@@ -1709,7 +1709,7 @@
   <dimension ref="B2:E45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.6"/>
@@ -1729,7 +1729,7 @@
     </row>
     <row r="4" spans="2:5">
       <c r="C4" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="2:5" s="2" customFormat="1">
@@ -1758,7 +1758,7 @@
         <v>50</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="2:5" s="1" customFormat="1">
@@ -1768,7 +1768,7 @@
     </row>
     <row r="13" spans="2:5">
       <c r="C13" s="3" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="2:5" s="2" customFormat="1">
@@ -1797,7 +1797,7 @@
         <v>50</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="2:5" s="1" customFormat="1">
@@ -1807,7 +1807,7 @@
     </row>
     <row r="22" spans="2:5">
       <c r="C22" s="3" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="24" spans="2:5" s="2" customFormat="1">
@@ -1833,10 +1833,10 @@
     <row r="27" spans="2:5">
       <c r="C27" s="6"/>
       <c r="D27" s="8" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="2:5" s="1" customFormat="1">
@@ -1846,7 +1846,7 @@
     </row>
     <row r="31" spans="2:5">
       <c r="C31" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="33" spans="2:5" s="2" customFormat="1">
@@ -1913,10 +1913,10 @@
     <row r="45" spans="2:5">
       <c r="C45" s="6"/>
       <c r="D45" s="8" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>